<commit_message>
Updating index tab templates
</commit_message>
<xml_diff>
--- a/Index Tab Templates.xlsx
+++ b/Index Tab Templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/GitHub/WormTracker3000/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC15C0B0-FF75-5648-B35B-F2186D105805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988DE58E-571E-A84F-AEC3-108DE8BA15E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2760" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{44AF9F45-7CA7-644B-9388-3D32C27F2940}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Number of Worms</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>OdorYCoord</t>
+  </si>
+  <si>
+    <t>Low gradient</t>
+  </si>
+  <si>
+    <t>High gradient</t>
+  </si>
+  <si>
+    <t>Distance between</t>
+  </si>
+  <si>
+    <t>Gradient slope (value per per cm)</t>
+  </si>
+  <si>
+    <t>Alignment distance</t>
   </si>
 </sst>
 </file>
@@ -585,10 +600,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D6BB2C-B31E-A746-B259-48CD095D3B64}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,11 +611,17 @@
     <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,30 +632,48 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding thermotaxis assay quantification
</commit_message>
<xml_diff>
--- a/Index Tab Templates.xlsx
+++ b/Index Tab Templates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/GitHub/WormTracker3000/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988DE58E-571E-A84F-AEC3-108DE8BA15E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE9A5E4-3B27-7447-A127-1EB8D7C9C51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2760" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{44AF9F45-7CA7-644B-9388-3D32C27F2940}"/>
+    <workbookView xWindow="4960" yWindow="3060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{44AF9F45-7CA7-644B-9388-3D32C27F2940}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemotaxis Index" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Number of Worms</t>
   </si>
@@ -56,22 +56,7 @@
     <t>UID</t>
   </si>
   <si>
-    <t>Tstart Camera</t>
-  </si>
-  <si>
-    <t>cmperdeg</t>
-  </si>
-  <si>
     <t>T(start)</t>
-  </si>
-  <si>
-    <t>CL pixels per cm</t>
-  </si>
-  <si>
-    <t>CR pixels per cm</t>
-  </si>
-  <si>
-    <t>T(odor)</t>
   </si>
   <si>
     <t>OdorXCoord</t>
@@ -531,10 +516,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E9F6C1-2DAD-D24D-BBD4-C630CBA3E617}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,11 +529,11 @@
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,41 +541,39 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -602,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D6BB2C-B31E-A746-B259-48CD095D3B64}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -632,16 +615,16 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -656,7 +639,7 @@
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>

</xml_diff>